<commit_message>
Updated .xlsx files with tables.
</commit_message>
<xml_diff>
--- a/data/CERES_Mehmood_v5.xlsx
+++ b/data/CERES_Mehmood_v5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehmo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studies and Work\PhD (Crop Science)\Research Data\AgMIP Calibration\Phase 4\2. Excel Sheets and Tables\v5_Uploaded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB4182A-2E54-42E2-88B7-BDAFB9F1FDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B79ED4-AAB9-4362-9E7D-6067AB54FD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="1" r:id="rId1"/>
@@ -261,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
   <si>
     <t>Name of the observed or required variable</t>
   </si>
@@ -461,18 +461,6 @@
     <t>Standard grain N (%)</t>
   </si>
   <si>
-    <t>BBCH10</t>
-  </si>
-  <si>
-    <t>BBCH30</t>
-  </si>
-  <si>
-    <t>BBCH90</t>
-  </si>
-  <si>
-    <t>BBCH55</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -482,9 +470,6 @@
     <t>H#AM</t>
   </si>
   <si>
-    <t>HP%M</t>
-  </si>
-  <si>
     <t>FRWHCER1_1</t>
   </si>
   <si>
@@ -549,6 +534,27 @@
   </si>
   <si>
     <t>FRWHCER1_22</t>
+  </si>
+  <si>
+    <t>Zadok10</t>
+  </si>
+  <si>
+    <t>Zadok30</t>
+  </si>
+  <si>
+    <t>Zadok55</t>
+  </si>
+  <si>
+    <t>Zadok90</t>
+  </si>
+  <si>
+    <t>HP%M1</t>
+  </si>
+  <si>
+    <t>GN%MN</t>
+  </si>
+  <si>
+    <t>Minimum grain N (%)</t>
   </si>
 </sst>
 </file>
@@ -979,7 +985,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1012,10 +1018,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1026,10 +1032,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1040,10 +1046,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1054,10 +1060,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1082,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>63</v>
@@ -1110,7 +1116,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>63</v>
@@ -1138,7 +1144,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>59</v>
@@ -1189,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,7 +1521,7 @@
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1649,7 +1655,26 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:7" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="G9" s="8"/>
@@ -2147,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2170,7 +2195,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2178,7 +2203,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2186,7 +2211,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2194,7 +2219,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2202,7 +2227,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2210,7 +2235,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2218,7 +2243,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2226,7 +2251,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2234,7 +2259,7 @@
         <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2242,7 +2267,7 @@
         <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2250,7 +2275,7 @@
         <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2258,7 +2283,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2266,7 +2291,7 @@
         <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2274,7 +2299,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2282,7 +2307,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2290,7 +2315,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2298,7 +2323,7 @@
         <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -2306,7 +2331,7 @@
         <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -2314,7 +2339,7 @@
         <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2322,7 +2347,7 @@
         <v>65</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2330,7 +2355,7 @@
         <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2338,7 +2363,7 @@
         <v>69</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>